<commit_message>
additional years of information
</commit_message>
<xml_diff>
--- a/prep/CS_CP_HAB/hab_mangrove_extent_mse2019.xlsx
+++ b/prep/CS_CP_HAB/hab_mangrove_extent_mse2019.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Hurtadoyhurtado\carpeta compartida\PROYECTOS\CI IdSO MANABÍ Y SANTA ELENA\CAPAS DE DATOS\DATOS CRUDOS\BIODIVERSIDAD\HÁBITATS\DATOS CRUDOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karla\Documents\Github\mse\prep\CS_CP_HAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB3410B0-8EDE-4E30-BD3F-2E94432CFBA1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19755" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manglar total mse" sheetId="6" r:id="rId1"/>
@@ -21,14 +22,24 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">hab_mangrove_extent_mse!$A$1:$D$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">hab_mangrove_extent_mse!$A$1:$D$49</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="60">
   <si>
     <t>SANTA ELENA</t>
   </si>
@@ -213,7 +224,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -361,7 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -375,12 +386,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,17 +428,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,7 +468,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -586,6 +605,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3988-4217-AD38-2D8ECBC52BDC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -597,11 +621,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="380800800"/>
-        <c:axId val="380812000"/>
+        <c:axId val="165455264"/>
+        <c:axId val="165453632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="380800800"/>
+        <c:axId val="165455264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +668,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380812000"/>
+        <c:crossAx val="165453632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -652,7 +676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="380812000"/>
+        <c:axId val="165453632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,7 +725,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380800800"/>
+        <c:crossAx val="165455264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -750,7 +774,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -887,6 +911,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CCFF-4B71-991C-AA8BDD9D5BD8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -898,11 +927,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="35114256"/>
-        <c:axId val="35112016"/>
+        <c:axId val="242394992"/>
+        <c:axId val="242397712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="35114256"/>
+        <c:axId val="242394992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,7 +974,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35112016"/>
+        <c:crossAx val="242397712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -953,7 +982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35112016"/>
+        <c:axId val="242397712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1031,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35114256"/>
+        <c:crossAx val="242394992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1067,7 +1096,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1099,7 +1134,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1930,1531 +1971,1531 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:K29"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I31" sqref="D31:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="12"/>
-    <col min="2" max="2" width="13.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="20" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="12"/>
-    <col min="5" max="5" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="257" width="11.42578125" style="12"/>
-    <col min="258" max="258" width="13.28515625" style="12" customWidth="1"/>
-    <col min="259" max="259" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="11.42578125" style="12"/>
-    <col min="261" max="261" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="262" max="513" width="11.42578125" style="12"/>
-    <col min="514" max="514" width="13.28515625" style="12" customWidth="1"/>
-    <col min="515" max="515" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="516" max="516" width="11.42578125" style="12"/>
-    <col min="517" max="517" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="518" max="769" width="11.42578125" style="12"/>
-    <col min="770" max="770" width="13.28515625" style="12" customWidth="1"/>
-    <col min="771" max="771" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="772" max="772" width="11.42578125" style="12"/>
-    <col min="773" max="773" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="774" max="1025" width="11.42578125" style="12"/>
-    <col min="1026" max="1026" width="13.28515625" style="12" customWidth="1"/>
-    <col min="1027" max="1027" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1028" width="11.42578125" style="12"/>
-    <col min="1029" max="1029" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="1030" max="1281" width="11.42578125" style="12"/>
-    <col min="1282" max="1282" width="13.28515625" style="12" customWidth="1"/>
-    <col min="1283" max="1283" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1284" width="11.42578125" style="12"/>
-    <col min="1285" max="1285" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="1286" max="1537" width="11.42578125" style="12"/>
-    <col min="1538" max="1538" width="13.28515625" style="12" customWidth="1"/>
-    <col min="1539" max="1539" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1540" width="11.42578125" style="12"/>
-    <col min="1541" max="1541" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="1542" max="1793" width="11.42578125" style="12"/>
-    <col min="1794" max="1794" width="13.28515625" style="12" customWidth="1"/>
-    <col min="1795" max="1795" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1796" width="11.42578125" style="12"/>
-    <col min="1797" max="1797" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="1798" max="2049" width="11.42578125" style="12"/>
-    <col min="2050" max="2050" width="13.28515625" style="12" customWidth="1"/>
-    <col min="2051" max="2051" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2052" width="11.42578125" style="12"/>
-    <col min="2053" max="2053" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2054" max="2305" width="11.42578125" style="12"/>
-    <col min="2306" max="2306" width="13.28515625" style="12" customWidth="1"/>
-    <col min="2307" max="2307" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2308" width="11.42578125" style="12"/>
-    <col min="2309" max="2309" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2310" max="2561" width="11.42578125" style="12"/>
-    <col min="2562" max="2562" width="13.28515625" style="12" customWidth="1"/>
-    <col min="2563" max="2563" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2564" width="11.42578125" style="12"/>
-    <col min="2565" max="2565" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2566" max="2817" width="11.42578125" style="12"/>
-    <col min="2818" max="2818" width="13.28515625" style="12" customWidth="1"/>
-    <col min="2819" max="2819" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2820" width="11.42578125" style="12"/>
-    <col min="2821" max="2821" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2822" max="3073" width="11.42578125" style="12"/>
-    <col min="3074" max="3074" width="13.28515625" style="12" customWidth="1"/>
-    <col min="3075" max="3075" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3076" width="11.42578125" style="12"/>
-    <col min="3077" max="3077" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="3078" max="3329" width="11.42578125" style="12"/>
-    <col min="3330" max="3330" width="13.28515625" style="12" customWidth="1"/>
-    <col min="3331" max="3331" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3332" width="11.42578125" style="12"/>
-    <col min="3333" max="3333" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="3334" max="3585" width="11.42578125" style="12"/>
-    <col min="3586" max="3586" width="13.28515625" style="12" customWidth="1"/>
-    <col min="3587" max="3587" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3588" width="11.42578125" style="12"/>
-    <col min="3589" max="3589" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="3590" max="3841" width="11.42578125" style="12"/>
-    <col min="3842" max="3842" width="13.28515625" style="12" customWidth="1"/>
-    <col min="3843" max="3843" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3844" width="11.42578125" style="12"/>
-    <col min="3845" max="3845" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="3846" max="4097" width="11.42578125" style="12"/>
-    <col min="4098" max="4098" width="13.28515625" style="12" customWidth="1"/>
-    <col min="4099" max="4099" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4100" width="11.42578125" style="12"/>
-    <col min="4101" max="4101" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="4102" max="4353" width="11.42578125" style="12"/>
-    <col min="4354" max="4354" width="13.28515625" style="12" customWidth="1"/>
-    <col min="4355" max="4355" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4356" width="11.42578125" style="12"/>
-    <col min="4357" max="4357" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="4358" max="4609" width="11.42578125" style="12"/>
-    <col min="4610" max="4610" width="13.28515625" style="12" customWidth="1"/>
-    <col min="4611" max="4611" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4612" width="11.42578125" style="12"/>
-    <col min="4613" max="4613" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="4614" max="4865" width="11.42578125" style="12"/>
-    <col min="4866" max="4866" width="13.28515625" style="12" customWidth="1"/>
-    <col min="4867" max="4867" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4868" width="11.42578125" style="12"/>
-    <col min="4869" max="4869" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="4870" max="5121" width="11.42578125" style="12"/>
-    <col min="5122" max="5122" width="13.28515625" style="12" customWidth="1"/>
-    <col min="5123" max="5123" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5124" width="11.42578125" style="12"/>
-    <col min="5125" max="5125" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="5126" max="5377" width="11.42578125" style="12"/>
-    <col min="5378" max="5378" width="13.28515625" style="12" customWidth="1"/>
-    <col min="5379" max="5379" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5380" width="11.42578125" style="12"/>
-    <col min="5381" max="5381" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="5382" max="5633" width="11.42578125" style="12"/>
-    <col min="5634" max="5634" width="13.28515625" style="12" customWidth="1"/>
-    <col min="5635" max="5635" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5636" width="11.42578125" style="12"/>
-    <col min="5637" max="5637" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="5638" max="5889" width="11.42578125" style="12"/>
-    <col min="5890" max="5890" width="13.28515625" style="12" customWidth="1"/>
-    <col min="5891" max="5891" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5892" width="11.42578125" style="12"/>
-    <col min="5893" max="5893" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="5894" max="6145" width="11.42578125" style="12"/>
-    <col min="6146" max="6146" width="13.28515625" style="12" customWidth="1"/>
-    <col min="6147" max="6147" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6148" width="11.42578125" style="12"/>
-    <col min="6149" max="6149" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6150" max="6401" width="11.42578125" style="12"/>
-    <col min="6402" max="6402" width="13.28515625" style="12" customWidth="1"/>
-    <col min="6403" max="6403" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6404" width="11.42578125" style="12"/>
-    <col min="6405" max="6405" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6406" max="6657" width="11.42578125" style="12"/>
-    <col min="6658" max="6658" width="13.28515625" style="12" customWidth="1"/>
-    <col min="6659" max="6659" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6660" width="11.42578125" style="12"/>
-    <col min="6661" max="6661" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6662" max="6913" width="11.42578125" style="12"/>
-    <col min="6914" max="6914" width="13.28515625" style="12" customWidth="1"/>
-    <col min="6915" max="6915" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6916" width="11.42578125" style="12"/>
-    <col min="6917" max="6917" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6918" max="7169" width="11.42578125" style="12"/>
-    <col min="7170" max="7170" width="13.28515625" style="12" customWidth="1"/>
-    <col min="7171" max="7171" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7172" width="11.42578125" style="12"/>
-    <col min="7173" max="7173" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7174" max="7425" width="11.42578125" style="12"/>
-    <col min="7426" max="7426" width="13.28515625" style="12" customWidth="1"/>
-    <col min="7427" max="7427" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7428" width="11.42578125" style="12"/>
-    <col min="7429" max="7429" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7430" max="7681" width="11.42578125" style="12"/>
-    <col min="7682" max="7682" width="13.28515625" style="12" customWidth="1"/>
-    <col min="7683" max="7683" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7684" width="11.42578125" style="12"/>
-    <col min="7685" max="7685" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7686" max="7937" width="11.42578125" style="12"/>
-    <col min="7938" max="7938" width="13.28515625" style="12" customWidth="1"/>
-    <col min="7939" max="7939" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7940" width="11.42578125" style="12"/>
-    <col min="7941" max="7941" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7942" max="8193" width="11.42578125" style="12"/>
-    <col min="8194" max="8194" width="13.28515625" style="12" customWidth="1"/>
-    <col min="8195" max="8195" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8196" width="11.42578125" style="12"/>
-    <col min="8197" max="8197" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="8198" max="8449" width="11.42578125" style="12"/>
-    <col min="8450" max="8450" width="13.28515625" style="12" customWidth="1"/>
-    <col min="8451" max="8451" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8452" width="11.42578125" style="12"/>
-    <col min="8453" max="8453" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="8454" max="8705" width="11.42578125" style="12"/>
-    <col min="8706" max="8706" width="13.28515625" style="12" customWidth="1"/>
-    <col min="8707" max="8707" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8708" width="11.42578125" style="12"/>
-    <col min="8709" max="8709" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="8710" max="8961" width="11.42578125" style="12"/>
-    <col min="8962" max="8962" width="13.28515625" style="12" customWidth="1"/>
-    <col min="8963" max="8963" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8964" width="11.42578125" style="12"/>
-    <col min="8965" max="8965" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="8966" max="9217" width="11.42578125" style="12"/>
-    <col min="9218" max="9218" width="13.28515625" style="12" customWidth="1"/>
-    <col min="9219" max="9219" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9220" width="11.42578125" style="12"/>
-    <col min="9221" max="9221" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="9222" max="9473" width="11.42578125" style="12"/>
-    <col min="9474" max="9474" width="13.28515625" style="12" customWidth="1"/>
-    <col min="9475" max="9475" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9476" width="11.42578125" style="12"/>
-    <col min="9477" max="9477" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="9478" max="9729" width="11.42578125" style="12"/>
-    <col min="9730" max="9730" width="13.28515625" style="12" customWidth="1"/>
-    <col min="9731" max="9731" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9732" width="11.42578125" style="12"/>
-    <col min="9733" max="9733" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="9734" max="9985" width="11.42578125" style="12"/>
-    <col min="9986" max="9986" width="13.28515625" style="12" customWidth="1"/>
-    <col min="9987" max="9987" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="9988" max="9988" width="11.42578125" style="12"/>
-    <col min="9989" max="9989" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="9990" max="10241" width="11.42578125" style="12"/>
-    <col min="10242" max="10242" width="13.28515625" style="12" customWidth="1"/>
-    <col min="10243" max="10243" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10244" width="11.42578125" style="12"/>
-    <col min="10245" max="10245" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10246" max="10497" width="11.42578125" style="12"/>
-    <col min="10498" max="10498" width="13.28515625" style="12" customWidth="1"/>
-    <col min="10499" max="10499" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10500" width="11.42578125" style="12"/>
-    <col min="10501" max="10501" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10502" max="10753" width="11.42578125" style="12"/>
-    <col min="10754" max="10754" width="13.28515625" style="12" customWidth="1"/>
-    <col min="10755" max="10755" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10756" width="11.42578125" style="12"/>
-    <col min="10757" max="10757" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10758" max="11009" width="11.42578125" style="12"/>
-    <col min="11010" max="11010" width="13.28515625" style="12" customWidth="1"/>
-    <col min="11011" max="11011" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11012" width="11.42578125" style="12"/>
-    <col min="11013" max="11013" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11014" max="11265" width="11.42578125" style="12"/>
-    <col min="11266" max="11266" width="13.28515625" style="12" customWidth="1"/>
-    <col min="11267" max="11267" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11268" width="11.42578125" style="12"/>
-    <col min="11269" max="11269" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11270" max="11521" width="11.42578125" style="12"/>
-    <col min="11522" max="11522" width="13.28515625" style="12" customWidth="1"/>
-    <col min="11523" max="11523" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11524" width="11.42578125" style="12"/>
-    <col min="11525" max="11525" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11526" max="11777" width="11.42578125" style="12"/>
-    <col min="11778" max="11778" width="13.28515625" style="12" customWidth="1"/>
-    <col min="11779" max="11779" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11780" width="11.42578125" style="12"/>
-    <col min="11781" max="11781" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11782" max="12033" width="11.42578125" style="12"/>
-    <col min="12034" max="12034" width="13.28515625" style="12" customWidth="1"/>
-    <col min="12035" max="12035" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12036" width="11.42578125" style="12"/>
-    <col min="12037" max="12037" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12038" max="12289" width="11.42578125" style="12"/>
-    <col min="12290" max="12290" width="13.28515625" style="12" customWidth="1"/>
-    <col min="12291" max="12291" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12292" width="11.42578125" style="12"/>
-    <col min="12293" max="12293" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12294" max="12545" width="11.42578125" style="12"/>
-    <col min="12546" max="12546" width="13.28515625" style="12" customWidth="1"/>
-    <col min="12547" max="12547" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12548" width="11.42578125" style="12"/>
-    <col min="12549" max="12549" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12550" max="12801" width="11.42578125" style="12"/>
-    <col min="12802" max="12802" width="13.28515625" style="12" customWidth="1"/>
-    <col min="12803" max="12803" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12804" width="11.42578125" style="12"/>
-    <col min="12805" max="12805" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12806" max="13057" width="11.42578125" style="12"/>
-    <col min="13058" max="13058" width="13.28515625" style="12" customWidth="1"/>
-    <col min="13059" max="13059" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13060" width="11.42578125" style="12"/>
-    <col min="13061" max="13061" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="13062" max="13313" width="11.42578125" style="12"/>
-    <col min="13314" max="13314" width="13.28515625" style="12" customWidth="1"/>
-    <col min="13315" max="13315" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13316" width="11.42578125" style="12"/>
-    <col min="13317" max="13317" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="13318" max="13569" width="11.42578125" style="12"/>
-    <col min="13570" max="13570" width="13.28515625" style="12" customWidth="1"/>
-    <col min="13571" max="13571" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13572" width="11.42578125" style="12"/>
-    <col min="13573" max="13573" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="13574" max="13825" width="11.42578125" style="12"/>
-    <col min="13826" max="13826" width="13.28515625" style="12" customWidth="1"/>
-    <col min="13827" max="13827" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13828" width="11.42578125" style="12"/>
-    <col min="13829" max="13829" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="13830" max="14081" width="11.42578125" style="12"/>
-    <col min="14082" max="14082" width="13.28515625" style="12" customWidth="1"/>
-    <col min="14083" max="14083" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14084" width="11.42578125" style="12"/>
-    <col min="14085" max="14085" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="14086" max="14337" width="11.42578125" style="12"/>
-    <col min="14338" max="14338" width="13.28515625" style="12" customWidth="1"/>
-    <col min="14339" max="14339" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14340" width="11.42578125" style="12"/>
-    <col min="14341" max="14341" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="14342" max="14593" width="11.42578125" style="12"/>
-    <col min="14594" max="14594" width="13.28515625" style="12" customWidth="1"/>
-    <col min="14595" max="14595" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14596" width="11.42578125" style="12"/>
-    <col min="14597" max="14597" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="14598" max="14849" width="11.42578125" style="12"/>
-    <col min="14850" max="14850" width="13.28515625" style="12" customWidth="1"/>
-    <col min="14851" max="14851" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14852" width="11.42578125" style="12"/>
-    <col min="14853" max="14853" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="14854" max="15105" width="11.42578125" style="12"/>
-    <col min="15106" max="15106" width="13.28515625" style="12" customWidth="1"/>
-    <col min="15107" max="15107" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15108" width="11.42578125" style="12"/>
-    <col min="15109" max="15109" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="15110" max="15361" width="11.42578125" style="12"/>
-    <col min="15362" max="15362" width="13.28515625" style="12" customWidth="1"/>
-    <col min="15363" max="15363" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15364" width="11.42578125" style="12"/>
-    <col min="15365" max="15365" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="15366" max="15617" width="11.42578125" style="12"/>
-    <col min="15618" max="15618" width="13.28515625" style="12" customWidth="1"/>
-    <col min="15619" max="15619" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15620" width="11.42578125" style="12"/>
-    <col min="15621" max="15621" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="15622" max="15873" width="11.42578125" style="12"/>
-    <col min="15874" max="15874" width="13.28515625" style="12" customWidth="1"/>
-    <col min="15875" max="15875" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15876" width="11.42578125" style="12"/>
-    <col min="15877" max="15877" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="15878" max="16129" width="11.42578125" style="12"/>
-    <col min="16130" max="16130" width="13.28515625" style="12" customWidth="1"/>
-    <col min="16131" max="16131" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16132" width="11.42578125" style="12"/>
-    <col min="16133" max="16133" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="16134" max="16384" width="11.42578125" style="12"/>
+    <col min="1" max="1" width="11.42578125" style="10"/>
+    <col min="2" max="2" width="13.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="20" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="10"/>
+    <col min="5" max="5" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="257" width="11.42578125" style="10"/>
+    <col min="258" max="258" width="13.28515625" style="10" customWidth="1"/>
+    <col min="259" max="259" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="11.42578125" style="10"/>
+    <col min="261" max="261" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="262" max="513" width="11.42578125" style="10"/>
+    <col min="514" max="514" width="13.28515625" style="10" customWidth="1"/>
+    <col min="515" max="515" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="516" max="516" width="11.42578125" style="10"/>
+    <col min="517" max="517" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="518" max="769" width="11.42578125" style="10"/>
+    <col min="770" max="770" width="13.28515625" style="10" customWidth="1"/>
+    <col min="771" max="771" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="772" max="772" width="11.42578125" style="10"/>
+    <col min="773" max="773" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="774" max="1025" width="11.42578125" style="10"/>
+    <col min="1026" max="1026" width="13.28515625" style="10" customWidth="1"/>
+    <col min="1027" max="1027" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="1028" max="1028" width="11.42578125" style="10"/>
+    <col min="1029" max="1029" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1030" max="1281" width="11.42578125" style="10"/>
+    <col min="1282" max="1282" width="13.28515625" style="10" customWidth="1"/>
+    <col min="1283" max="1283" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="1284" max="1284" width="11.42578125" style="10"/>
+    <col min="1285" max="1285" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1286" max="1537" width="11.42578125" style="10"/>
+    <col min="1538" max="1538" width="13.28515625" style="10" customWidth="1"/>
+    <col min="1539" max="1539" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="1540" max="1540" width="11.42578125" style="10"/>
+    <col min="1541" max="1541" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1542" max="1793" width="11.42578125" style="10"/>
+    <col min="1794" max="1794" width="13.28515625" style="10" customWidth="1"/>
+    <col min="1795" max="1795" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="1796" max="1796" width="11.42578125" style="10"/>
+    <col min="1797" max="1797" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1798" max="2049" width="11.42578125" style="10"/>
+    <col min="2050" max="2050" width="13.28515625" style="10" customWidth="1"/>
+    <col min="2051" max="2051" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="2052" max="2052" width="11.42578125" style="10"/>
+    <col min="2053" max="2053" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2054" max="2305" width="11.42578125" style="10"/>
+    <col min="2306" max="2306" width="13.28515625" style="10" customWidth="1"/>
+    <col min="2307" max="2307" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="2308" max="2308" width="11.42578125" style="10"/>
+    <col min="2309" max="2309" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2310" max="2561" width="11.42578125" style="10"/>
+    <col min="2562" max="2562" width="13.28515625" style="10" customWidth="1"/>
+    <col min="2563" max="2563" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="2564" max="2564" width="11.42578125" style="10"/>
+    <col min="2565" max="2565" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2566" max="2817" width="11.42578125" style="10"/>
+    <col min="2818" max="2818" width="13.28515625" style="10" customWidth="1"/>
+    <col min="2819" max="2819" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="2820" max="2820" width="11.42578125" style="10"/>
+    <col min="2821" max="2821" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2822" max="3073" width="11.42578125" style="10"/>
+    <col min="3074" max="3074" width="13.28515625" style="10" customWidth="1"/>
+    <col min="3075" max="3075" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="3076" max="3076" width="11.42578125" style="10"/>
+    <col min="3077" max="3077" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3078" max="3329" width="11.42578125" style="10"/>
+    <col min="3330" max="3330" width="13.28515625" style="10" customWidth="1"/>
+    <col min="3331" max="3331" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="3332" max="3332" width="11.42578125" style="10"/>
+    <col min="3333" max="3333" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3334" max="3585" width="11.42578125" style="10"/>
+    <col min="3586" max="3586" width="13.28515625" style="10" customWidth="1"/>
+    <col min="3587" max="3587" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="3588" max="3588" width="11.42578125" style="10"/>
+    <col min="3589" max="3589" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3590" max="3841" width="11.42578125" style="10"/>
+    <col min="3842" max="3842" width="13.28515625" style="10" customWidth="1"/>
+    <col min="3843" max="3843" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="3844" max="3844" width="11.42578125" style="10"/>
+    <col min="3845" max="3845" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3846" max="4097" width="11.42578125" style="10"/>
+    <col min="4098" max="4098" width="13.28515625" style="10" customWidth="1"/>
+    <col min="4099" max="4099" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="4100" max="4100" width="11.42578125" style="10"/>
+    <col min="4101" max="4101" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4102" max="4353" width="11.42578125" style="10"/>
+    <col min="4354" max="4354" width="13.28515625" style="10" customWidth="1"/>
+    <col min="4355" max="4355" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="4356" max="4356" width="11.42578125" style="10"/>
+    <col min="4357" max="4357" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4358" max="4609" width="11.42578125" style="10"/>
+    <col min="4610" max="4610" width="13.28515625" style="10" customWidth="1"/>
+    <col min="4611" max="4611" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="4612" max="4612" width="11.42578125" style="10"/>
+    <col min="4613" max="4613" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4614" max="4865" width="11.42578125" style="10"/>
+    <col min="4866" max="4866" width="13.28515625" style="10" customWidth="1"/>
+    <col min="4867" max="4867" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="4868" max="4868" width="11.42578125" style="10"/>
+    <col min="4869" max="4869" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4870" max="5121" width="11.42578125" style="10"/>
+    <col min="5122" max="5122" width="13.28515625" style="10" customWidth="1"/>
+    <col min="5123" max="5123" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="5124" max="5124" width="11.42578125" style="10"/>
+    <col min="5125" max="5125" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5126" max="5377" width="11.42578125" style="10"/>
+    <col min="5378" max="5378" width="13.28515625" style="10" customWidth="1"/>
+    <col min="5379" max="5379" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="5380" max="5380" width="11.42578125" style="10"/>
+    <col min="5381" max="5381" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5382" max="5633" width="11.42578125" style="10"/>
+    <col min="5634" max="5634" width="13.28515625" style="10" customWidth="1"/>
+    <col min="5635" max="5635" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="5636" max="5636" width="11.42578125" style="10"/>
+    <col min="5637" max="5637" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5638" max="5889" width="11.42578125" style="10"/>
+    <col min="5890" max="5890" width="13.28515625" style="10" customWidth="1"/>
+    <col min="5891" max="5891" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="5892" max="5892" width="11.42578125" style="10"/>
+    <col min="5893" max="5893" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5894" max="6145" width="11.42578125" style="10"/>
+    <col min="6146" max="6146" width="13.28515625" style="10" customWidth="1"/>
+    <col min="6147" max="6147" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="6148" max="6148" width="11.42578125" style="10"/>
+    <col min="6149" max="6149" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6150" max="6401" width="11.42578125" style="10"/>
+    <col min="6402" max="6402" width="13.28515625" style="10" customWidth="1"/>
+    <col min="6403" max="6403" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="6404" max="6404" width="11.42578125" style="10"/>
+    <col min="6405" max="6405" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6406" max="6657" width="11.42578125" style="10"/>
+    <col min="6658" max="6658" width="13.28515625" style="10" customWidth="1"/>
+    <col min="6659" max="6659" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="6660" max="6660" width="11.42578125" style="10"/>
+    <col min="6661" max="6661" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6662" max="6913" width="11.42578125" style="10"/>
+    <col min="6914" max="6914" width="13.28515625" style="10" customWidth="1"/>
+    <col min="6915" max="6915" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="6916" max="6916" width="11.42578125" style="10"/>
+    <col min="6917" max="6917" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6918" max="7169" width="11.42578125" style="10"/>
+    <col min="7170" max="7170" width="13.28515625" style="10" customWidth="1"/>
+    <col min="7171" max="7171" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="7172" max="7172" width="11.42578125" style="10"/>
+    <col min="7173" max="7173" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7174" max="7425" width="11.42578125" style="10"/>
+    <col min="7426" max="7426" width="13.28515625" style="10" customWidth="1"/>
+    <col min="7427" max="7427" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="7428" max="7428" width="11.42578125" style="10"/>
+    <col min="7429" max="7429" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7430" max="7681" width="11.42578125" style="10"/>
+    <col min="7682" max="7682" width="13.28515625" style="10" customWidth="1"/>
+    <col min="7683" max="7683" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="7684" max="7684" width="11.42578125" style="10"/>
+    <col min="7685" max="7685" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7686" max="7937" width="11.42578125" style="10"/>
+    <col min="7938" max="7938" width="13.28515625" style="10" customWidth="1"/>
+    <col min="7939" max="7939" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="7940" max="7940" width="11.42578125" style="10"/>
+    <col min="7941" max="7941" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7942" max="8193" width="11.42578125" style="10"/>
+    <col min="8194" max="8194" width="13.28515625" style="10" customWidth="1"/>
+    <col min="8195" max="8195" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="8196" max="8196" width="11.42578125" style="10"/>
+    <col min="8197" max="8197" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8198" max="8449" width="11.42578125" style="10"/>
+    <col min="8450" max="8450" width="13.28515625" style="10" customWidth="1"/>
+    <col min="8451" max="8451" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="8452" max="8452" width="11.42578125" style="10"/>
+    <col min="8453" max="8453" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8454" max="8705" width="11.42578125" style="10"/>
+    <col min="8706" max="8706" width="13.28515625" style="10" customWidth="1"/>
+    <col min="8707" max="8707" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="8708" max="8708" width="11.42578125" style="10"/>
+    <col min="8709" max="8709" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8710" max="8961" width="11.42578125" style="10"/>
+    <col min="8962" max="8962" width="13.28515625" style="10" customWidth="1"/>
+    <col min="8963" max="8963" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="8964" max="8964" width="11.42578125" style="10"/>
+    <col min="8965" max="8965" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8966" max="9217" width="11.42578125" style="10"/>
+    <col min="9218" max="9218" width="13.28515625" style="10" customWidth="1"/>
+    <col min="9219" max="9219" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="9220" max="9220" width="11.42578125" style="10"/>
+    <col min="9221" max="9221" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9222" max="9473" width="11.42578125" style="10"/>
+    <col min="9474" max="9474" width="13.28515625" style="10" customWidth="1"/>
+    <col min="9475" max="9475" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="9476" max="9476" width="11.42578125" style="10"/>
+    <col min="9477" max="9477" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9478" max="9729" width="11.42578125" style="10"/>
+    <col min="9730" max="9730" width="13.28515625" style="10" customWidth="1"/>
+    <col min="9731" max="9731" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="9732" max="9732" width="11.42578125" style="10"/>
+    <col min="9733" max="9733" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9734" max="9985" width="11.42578125" style="10"/>
+    <col min="9986" max="9986" width="13.28515625" style="10" customWidth="1"/>
+    <col min="9987" max="9987" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="9988" max="9988" width="11.42578125" style="10"/>
+    <col min="9989" max="9989" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9990" max="10241" width="11.42578125" style="10"/>
+    <col min="10242" max="10242" width="13.28515625" style="10" customWidth="1"/>
+    <col min="10243" max="10243" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="10244" max="10244" width="11.42578125" style="10"/>
+    <col min="10245" max="10245" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10246" max="10497" width="11.42578125" style="10"/>
+    <col min="10498" max="10498" width="13.28515625" style="10" customWidth="1"/>
+    <col min="10499" max="10499" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="10500" max="10500" width="11.42578125" style="10"/>
+    <col min="10501" max="10501" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10502" max="10753" width="11.42578125" style="10"/>
+    <col min="10754" max="10754" width="13.28515625" style="10" customWidth="1"/>
+    <col min="10755" max="10755" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="10756" max="10756" width="11.42578125" style="10"/>
+    <col min="10757" max="10757" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10758" max="11009" width="11.42578125" style="10"/>
+    <col min="11010" max="11010" width="13.28515625" style="10" customWidth="1"/>
+    <col min="11011" max="11011" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="11012" max="11012" width="11.42578125" style="10"/>
+    <col min="11013" max="11013" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11014" max="11265" width="11.42578125" style="10"/>
+    <col min="11266" max="11266" width="13.28515625" style="10" customWidth="1"/>
+    <col min="11267" max="11267" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="11268" max="11268" width="11.42578125" style="10"/>
+    <col min="11269" max="11269" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11270" max="11521" width="11.42578125" style="10"/>
+    <col min="11522" max="11522" width="13.28515625" style="10" customWidth="1"/>
+    <col min="11523" max="11523" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="11524" max="11524" width="11.42578125" style="10"/>
+    <col min="11525" max="11525" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11526" max="11777" width="11.42578125" style="10"/>
+    <col min="11778" max="11778" width="13.28515625" style="10" customWidth="1"/>
+    <col min="11779" max="11779" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="11780" max="11780" width="11.42578125" style="10"/>
+    <col min="11781" max="11781" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11782" max="12033" width="11.42578125" style="10"/>
+    <col min="12034" max="12034" width="13.28515625" style="10" customWidth="1"/>
+    <col min="12035" max="12035" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="12036" max="12036" width="11.42578125" style="10"/>
+    <col min="12037" max="12037" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12038" max="12289" width="11.42578125" style="10"/>
+    <col min="12290" max="12290" width="13.28515625" style="10" customWidth="1"/>
+    <col min="12291" max="12291" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="12292" max="12292" width="11.42578125" style="10"/>
+    <col min="12293" max="12293" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12294" max="12545" width="11.42578125" style="10"/>
+    <col min="12546" max="12546" width="13.28515625" style="10" customWidth="1"/>
+    <col min="12547" max="12547" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="12548" max="12548" width="11.42578125" style="10"/>
+    <col min="12549" max="12549" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12550" max="12801" width="11.42578125" style="10"/>
+    <col min="12802" max="12802" width="13.28515625" style="10" customWidth="1"/>
+    <col min="12803" max="12803" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="12804" max="12804" width="11.42578125" style="10"/>
+    <col min="12805" max="12805" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12806" max="13057" width="11.42578125" style="10"/>
+    <col min="13058" max="13058" width="13.28515625" style="10" customWidth="1"/>
+    <col min="13059" max="13059" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="13060" max="13060" width="11.42578125" style="10"/>
+    <col min="13061" max="13061" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13062" max="13313" width="11.42578125" style="10"/>
+    <col min="13314" max="13314" width="13.28515625" style="10" customWidth="1"/>
+    <col min="13315" max="13315" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="13316" max="13316" width="11.42578125" style="10"/>
+    <col min="13317" max="13317" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13318" max="13569" width="11.42578125" style="10"/>
+    <col min="13570" max="13570" width="13.28515625" style="10" customWidth="1"/>
+    <col min="13571" max="13571" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="13572" max="13572" width="11.42578125" style="10"/>
+    <col min="13573" max="13573" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13574" max="13825" width="11.42578125" style="10"/>
+    <col min="13826" max="13826" width="13.28515625" style="10" customWidth="1"/>
+    <col min="13827" max="13827" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="13828" max="13828" width="11.42578125" style="10"/>
+    <col min="13829" max="13829" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13830" max="14081" width="11.42578125" style="10"/>
+    <col min="14082" max="14082" width="13.28515625" style="10" customWidth="1"/>
+    <col min="14083" max="14083" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="14084" max="14084" width="11.42578125" style="10"/>
+    <col min="14085" max="14085" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="14086" max="14337" width="11.42578125" style="10"/>
+    <col min="14338" max="14338" width="13.28515625" style="10" customWidth="1"/>
+    <col min="14339" max="14339" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="14340" max="14340" width="11.42578125" style="10"/>
+    <col min="14341" max="14341" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="14342" max="14593" width="11.42578125" style="10"/>
+    <col min="14594" max="14594" width="13.28515625" style="10" customWidth="1"/>
+    <col min="14595" max="14595" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="14596" max="14596" width="11.42578125" style="10"/>
+    <col min="14597" max="14597" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="14598" max="14849" width="11.42578125" style="10"/>
+    <col min="14850" max="14850" width="13.28515625" style="10" customWidth="1"/>
+    <col min="14851" max="14851" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="14852" max="14852" width="11.42578125" style="10"/>
+    <col min="14853" max="14853" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="14854" max="15105" width="11.42578125" style="10"/>
+    <col min="15106" max="15106" width="13.28515625" style="10" customWidth="1"/>
+    <col min="15107" max="15107" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="15108" max="15108" width="11.42578125" style="10"/>
+    <col min="15109" max="15109" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15110" max="15361" width="11.42578125" style="10"/>
+    <col min="15362" max="15362" width="13.28515625" style="10" customWidth="1"/>
+    <col min="15363" max="15363" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="15364" max="15364" width="11.42578125" style="10"/>
+    <col min="15365" max="15365" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15366" max="15617" width="11.42578125" style="10"/>
+    <col min="15618" max="15618" width="13.28515625" style="10" customWidth="1"/>
+    <col min="15619" max="15619" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="15620" max="15620" width="11.42578125" style="10"/>
+    <col min="15621" max="15621" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15622" max="15873" width="11.42578125" style="10"/>
+    <col min="15874" max="15874" width="13.28515625" style="10" customWidth="1"/>
+    <col min="15875" max="15875" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="15876" max="15876" width="11.42578125" style="10"/>
+    <col min="15877" max="15877" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15878" max="16129" width="11.42578125" style="10"/>
+    <col min="16130" max="16130" width="13.28515625" style="10" customWidth="1"/>
+    <col min="16131" max="16131" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="16132" max="16132" width="11.42578125" style="10"/>
+    <col min="16133" max="16133" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="16134" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
+      <c r="A2" s="10">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="10">
         <f>[1]zonas!D42</f>
         <v>0</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="10">
         <f>[1]zonas!E42</f>
         <v>0</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="10">
         <f>[1]zonas!F42</f>
         <v>0</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="10">
         <f>[1]zonas!G42</f>
         <v>0</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="10">
         <f>[1]zonas!H42</f>
         <v>0</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="10">
         <f>[1]zonas!I42</f>
         <v>0</v>
       </c>
-      <c r="J2" s="12">
+      <c r="J2" s="10">
         <f>[1]zonas!J42</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="13"/>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="10">
         <f>[1]zonas!D46</f>
         <v>0</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="10">
         <f>[1]zonas!E46</f>
         <v>0</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="10">
         <f>[1]zonas!F46</f>
         <v>0</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="10">
         <f>[1]zonas!G46</f>
         <v>0</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="10">
         <f>[1]zonas!H46</f>
         <v>0</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="10">
         <f>[1]zonas!I46</f>
         <v>0</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="10">
         <f>[1]zonas!J46</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="13"/>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <f>[1]zonas!D128</f>
         <v>144</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <f>[1]zonas!E128</f>
         <v>144.19999999999999</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <f>[1]zonas!F128</f>
         <v>144.19999999999999</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="10">
         <f>[1]zonas!G128</f>
         <v>144.19999999999999</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="10">
         <f>[1]zonas!H128</f>
         <v>128.6</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="10">
         <f>[1]zonas!I128</f>
         <v>36.86</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="10">
         <f>[1]zonas!J128</f>
         <v>32.141306999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="15"/>
-      <c r="C5" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9">
+    <row r="5" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
         <f>SUM(D2:D4)</f>
         <v>144</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <f t="shared" ref="E5:J5" si="0">SUM(E2:E4)</f>
         <v>144.19999999999999</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <f t="shared" si="0"/>
         <v>144.19999999999999</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <f t="shared" si="0"/>
         <v>144.19999999999999</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="7">
         <f t="shared" si="0"/>
         <v>128.6</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <f t="shared" si="0"/>
         <v>36.86</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="15">
         <f t="shared" si="0"/>
         <v>32.141306999999998</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
+      <c r="A6" s="10">
         <v>7</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <f>[1]zonas!D22</f>
         <v>1392</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <f>[1]zonas!E22</f>
         <v>1003.8</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="16">
         <f>[1]zonas!F22</f>
         <v>1003.8</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="16">
         <f>[1]zonas!G22</f>
         <v>825.4</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="16">
         <f>[1]zonas!H22</f>
         <v>560.6</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="16">
         <f>[1]zonas!I22</f>
         <v>216.66</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="16">
         <f>[1]zonas!J22</f>
         <v>312.61490700000002</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <f>[1]zonas!D23</f>
         <v>494</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <f>[1]zonas!E23</f>
         <v>621.29999999999995</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="16">
         <f>[1]zonas!F23</f>
         <v>557.29999999999995</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="16">
         <f>[1]zonas!G23</f>
         <v>366.41</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="16">
         <f>[1]zonas!H23</f>
         <v>198.01</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <f>[1]zonas!I23</f>
         <v>154.55000000000001</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="16">
         <f>[1]zonas!J23</f>
         <v>167.649325</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <f>[1]zonas!D24</f>
         <v>374</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <f>[1]zonas!E24</f>
         <v>361.3</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="16">
         <f>[1]zonas!F24</f>
         <v>361.3</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="16">
         <f>[1]zonas!G24</f>
         <v>179.18</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="16">
         <f>[1]zonas!H24</f>
         <v>150.68</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="16">
         <f>[1]zonas!I24</f>
         <v>37.89</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="16">
         <f>[1]zonas!J24</f>
         <v>49.228422999999999</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <f>[1]zonas!D25</f>
         <v>1771</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="16">
         <f>[1]zonas!E25</f>
         <v>1421</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="16">
         <f>[1]zonas!F25</f>
         <v>1016.7</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="16">
         <f>[1]zonas!G25</f>
         <v>1678.15</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="16">
         <f>[1]zonas!H25</f>
         <v>1081.45</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="16">
         <f>[1]zonas!I25</f>
         <v>546.14</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="16">
         <f>[1]zonas!J25</f>
         <v>769.47629500000005</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <f>[1]zonas!D26</f>
         <v>683</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <f>[1]zonas!E26</f>
         <v>327.3</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="16">
         <f>[1]zonas!F26</f>
         <v>327.3</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="16">
         <f>[1]zonas!G26</f>
         <v>210.83</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="16">
         <f>[1]zonas!H26</f>
         <v>184.13</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="16">
         <f>[1]zonas!I26</f>
         <v>59.35</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="16">
         <f>[1]zonas!J26</f>
         <v>103.871298</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <f>[1]zonas!D27</f>
         <v>4197.5</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="16">
         <f>[1]zonas!E27</f>
         <v>3384.4</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <f>[1]zonas!F27</f>
         <v>2671.4</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="16">
         <f>[1]zonas!G27</f>
         <v>1976.8</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="16">
         <f>[1]zonas!H27</f>
         <v>1146.3</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="16">
         <f>[1]zonas!I27</f>
         <v>555.07000000000005</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="16">
         <f>[1]zonas!J27</f>
         <v>756.75719100000003</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <f>[1]zonas!D28</f>
         <v>509</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="16">
         <f>[1]zonas!E28</f>
         <v>273.3</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="16">
         <f>[1]zonas!F28</f>
         <v>183.3</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="16">
         <f>[1]zonas!G28</f>
         <v>162.30000000000001</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="16">
         <f>[1]zonas!H28</f>
         <v>146.5</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="16">
         <f>[1]zonas!I28</f>
         <v>32.61</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="16">
         <f>[1]zonas!J28</f>
         <v>81.074395999999993</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="16">
         <f>[1]zonas!D29</f>
         <v>800</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="16">
         <f>[1]zonas!E29</f>
         <v>415.6</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="16">
         <f>[1]zonas!F29</f>
         <v>334.1</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="16">
         <f>[1]zonas!G29</f>
         <v>227.39</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="16">
         <f>[1]zonas!H29</f>
         <v>71.39</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="16">
         <f>[1]zonas!I29</f>
         <v>69.2</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="16">
         <f>[1]zonas!J29</f>
         <v>183.164468</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="10">
         <f>[1]zonas!D32</f>
         <v>509</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="10">
         <f>[1]zonas!E32</f>
         <v>188</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="10">
         <f>[1]zonas!F32</f>
         <v>98.3</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="10">
         <f>[1]zonas!G32</f>
         <v>93.95</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="10">
         <f>[1]zonas!H32</f>
         <v>18.149999999999999</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="10">
         <f>[1]zonas!I32</f>
         <v>96.96</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="10">
         <f>[1]zonas!J32</f>
         <v>56.215190999999997</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="10">
         <f>[1]zonas!D33</f>
         <v>1884</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="10">
         <f>[1]zonas!E33</f>
         <v>851.6</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="10">
         <f>[1]zonas!F33</f>
         <v>475.7</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="10">
         <f>[1]zonas!G33</f>
         <v>338.47</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="10">
         <f>[1]zonas!H33</f>
         <v>157.47</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="10">
         <f>[1]zonas!I33</f>
         <v>337.4</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="10">
         <f>[1]zonas!J33</f>
         <v>545.70945700000004</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="10">
         <f>[1]zonas!D34</f>
         <v>1548</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="10">
         <f>[1]zonas!E34</f>
         <v>633.1</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="10">
         <f>[1]zonas!F34</f>
         <v>466</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="10">
         <f>[1]zonas!G34</f>
         <v>352.46</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="10">
         <f>[1]zonas!H34</f>
         <v>215.96</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="10">
         <f>[1]zonas!I34</f>
         <v>270.63</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="10">
         <f>[1]zonas!J34</f>
         <v>330.54091199999999</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="10">
         <f>[1]zonas!D119</f>
         <v>0</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="10">
         <f>[1]zonas!E119</f>
         <v>0</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="10">
         <f>[1]zonas!F119</f>
         <v>0</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="10">
         <f>[1]zonas!G119</f>
         <v>0</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="10">
         <f>[1]zonas!H119</f>
         <v>0</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="10">
         <f>[1]zonas!I119</f>
         <v>0</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="10">
         <f>[1]zonas!J119</f>
         <v>6.9592700000000001</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="16">
         <f>[1]zonas!D120</f>
         <v>54</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="16">
         <f>[1]zonas!E120</f>
         <v>22.5</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="16">
         <f>[1]zonas!F120</f>
         <v>22.5</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="16">
         <f>[1]zonas!G120</f>
         <v>22.5</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="16">
         <f>[1]zonas!H120</f>
         <v>21.3</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="16">
         <f>[1]zonas!I120</f>
         <v>3.42</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="16">
         <f>[1]zonas!J120</f>
         <v>4.0281909999999996</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="16">
         <f>[1]zonas!D121</f>
         <v>2</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="16">
         <f>[1]zonas!E121</f>
         <v>0</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="16">
         <f>[1]zonas!F121</f>
         <v>0</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="16">
         <f>[1]zonas!G121</f>
         <v>0</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="16">
         <f>[1]zonas!H121</f>
         <v>0</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="16">
         <f>[1]zonas!I121</f>
         <v>0</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="16">
         <f>[1]zonas!J121</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="16">
         <f>[1]zonas!D122</f>
         <v>18</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="16">
         <f>[1]zonas!E122</f>
         <v>18</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="16">
         <f>[1]zonas!F122</f>
         <v>18</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="16">
         <f>[1]zonas!G122</f>
         <v>15.38</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="16">
         <f>[1]zonas!H122</f>
         <v>5.08</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="16">
         <f>[1]zonas!I122</f>
         <v>0</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="16">
         <f>[1]zonas!J122</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="16">
         <f>[1]zonas!D123</f>
         <v>0</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="16">
         <f>[1]zonas!E123</f>
         <v>0</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="16">
         <f>[1]zonas!F123</f>
         <v>0</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="16">
         <f>[1]zonas!G123</f>
         <v>0</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="16">
         <f>[1]zonas!H123</f>
         <v>0</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="16">
         <f>[1]zonas!I123</f>
         <v>0</v>
       </c>
-      <c r="J21" s="18">
+      <c r="J21" s="16">
         <f>[1]zonas!J123</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="16">
         <f>[1]zonas!D124</f>
         <v>7</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="16">
         <f>[1]zonas!E124</f>
         <v>0</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="16">
         <f>[1]zonas!F124</f>
         <v>0</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="16">
         <f>[1]zonas!G124</f>
         <v>0</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H22" s="16">
         <f>[1]zonas!H124</f>
         <v>0</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I22" s="16">
         <f>[1]zonas!I124</f>
         <v>0</v>
       </c>
-      <c r="J22" s="18">
+      <c r="J22" s="16">
         <f>[1]zonas!J124</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="16">
         <f>[1]zonas!D125</f>
         <v>32</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="16">
         <f>[1]zonas!E125</f>
         <v>0</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="16">
         <f>[1]zonas!F125</f>
         <v>0</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="16">
         <f>[1]zonas!G125</f>
         <v>0</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H23" s="16">
         <f>[1]zonas!H125</f>
         <v>0</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I23" s="16">
         <f>[1]zonas!I125</f>
         <v>0</v>
       </c>
-      <c r="J23" s="18">
+      <c r="J23" s="16">
         <f>[1]zonas!J125</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="16">
         <f>[1]zonas!D126</f>
         <v>83</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="16">
         <f>[1]zonas!E126</f>
         <v>81.3</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="16">
         <f>[1]zonas!F126</f>
         <v>81.3</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="16">
         <f>[1]zonas!G126</f>
         <v>81.3</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="16">
         <f>[1]zonas!H126</f>
         <v>81.3</v>
       </c>
-      <c r="I24" s="18">
+      <c r="I24" s="16">
         <f>[1]zonas!I126</f>
         <v>35.01</v>
       </c>
-      <c r="J24" s="18">
+      <c r="J24" s="16">
         <f>[1]zonas!J126</f>
         <v>35.005983999999998</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="16">
         <f>[1]zonas!D127</f>
         <v>0</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="16">
         <f>[1]zonas!E127</f>
         <v>0</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="16">
         <f>[1]zonas!F127</f>
         <v>0</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="16">
         <f>[1]zonas!G127</f>
         <v>0</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="16">
         <f>[1]zonas!H127</f>
         <v>0</v>
       </c>
-      <c r="I25" s="18">
+      <c r="I25" s="16">
         <f>[1]zonas!I127</f>
         <v>0</v>
       </c>
-      <c r="J25" s="18">
+      <c r="J25" s="16">
         <f>[1]zonas!J127</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="10" t="s">
+    <row r="26" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="18">
         <f>SUM(D6:D25)</f>
         <v>14357.5</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="18">
         <f t="shared" ref="E26:J26" si="1">SUM(E6:E25)</f>
         <v>9602.5</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="18">
         <f t="shared" si="1"/>
         <v>7617.0000000000009</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="18">
         <f t="shared" si="1"/>
         <v>6530.5200000000013</v>
       </c>
-      <c r="H26" s="20">
+      <c r="H26" s="18">
         <f t="shared" si="1"/>
         <v>4038.32</v>
       </c>
-      <c r="I26" s="20">
+      <c r="I26" s="18">
         <f t="shared" si="1"/>
         <v>2414.8900000000003</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="18">
         <f t="shared" si="1"/>
         <v>3402.2953079999993</v>
       </c>
     </row>
     <row r="28" spans="2:11" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="11" t="s">
+      <c r="I28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J28" s="11" t="s">
+      <c r="J28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K28" s="11" t="s">
+      <c r="K28" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="J29" s="11" t="s">
+      <c r="J29" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="K29" s="11" t="s">
+      <c r="K29" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="12">
+      <c r="B30" s="10">
         <v>6</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="21">
         <f t="shared" ref="D30:J30" si="2">D5/100</f>
         <v>1.44</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="21">
         <f t="shared" si="2"/>
         <v>1.4419999999999999</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="21">
         <f t="shared" si="2"/>
         <v>1.4419999999999999</v>
       </c>
-      <c r="G30" s="23">
+      <c r="G30" s="21">
         <f t="shared" si="2"/>
         <v>1.4419999999999999</v>
       </c>
-      <c r="H30" s="23">
+      <c r="H30" s="21">
         <f t="shared" si="2"/>
         <v>1.286</v>
       </c>
-      <c r="I30" s="23">
+      <c r="I30" s="21">
         <f t="shared" si="2"/>
         <v>0.36859999999999998</v>
       </c>
-      <c r="J30" s="23">
+      <c r="J30" s="21">
         <f t="shared" si="2"/>
         <v>0.32141306999999997</v>
       </c>
-      <c r="K30" s="24">
+      <c r="K30" s="22">
         <f>[2]Hoja1!$E$5</f>
         <v>0.30224000000000001</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="12">
+      <c r="B31" s="10">
         <v>7</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="23">
+      <c r="D31" s="21">
         <f t="shared" ref="D31:J31" si="3">D26/100</f>
         <v>143.57499999999999</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="21">
         <f t="shared" si="3"/>
         <v>96.025000000000006</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="21">
         <f t="shared" si="3"/>
         <v>76.170000000000016</v>
       </c>
-      <c r="G31" s="23">
+      <c r="G31" s="21">
         <f t="shared" si="3"/>
         <v>65.305200000000013</v>
       </c>
-      <c r="H31" s="23">
+      <c r="H31" s="21">
         <f t="shared" si="3"/>
         <v>40.383200000000002</v>
       </c>
-      <c r="I31" s="23">
+      <c r="I31" s="21">
         <f t="shared" si="3"/>
         <v>24.148900000000005</v>
       </c>
-      <c r="J31" s="23">
+      <c r="J31" s="21">
         <f t="shared" si="3"/>
         <v>34.022953079999994</v>
       </c>
-      <c r="K31" s="24">
+      <c r="K31" s="22">
         <f>[2]Hoja1!$E$6</f>
         <v>28.045209</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D32" s="23">
+      <c r="D32" s="21">
         <f t="shared" ref="D32:K32" si="4">SUM(D30:D31)</f>
         <v>145.01499999999999</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <f t="shared" si="4"/>
         <v>97.466999999999999</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="21">
         <f t="shared" si="4"/>
         <v>77.612000000000009</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="21">
         <f t="shared" si="4"/>
         <v>66.747200000000007</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H32" s="21">
         <f t="shared" si="4"/>
         <v>41.669200000000004</v>
       </c>
-      <c r="I32" s="23">
+      <c r="I32" s="21">
         <f t="shared" si="4"/>
         <v>24.517500000000005</v>
       </c>
-      <c r="J32" s="23">
+      <c r="J32" s="21">
         <f t="shared" si="4"/>
         <v>34.344366149999992</v>
       </c>
-      <c r="K32" s="24">
+      <c r="K32" s="22">
         <f t="shared" si="4"/>
         <v>28.347449000000001</v>
       </c>
     </row>
     <row r="34" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D34" s="25"/>
-      <c r="E34" s="25" t="s">
+      <c r="D34" s="23"/>
+      <c r="E34" s="23" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="35" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D35" s="26"/>
-      <c r="E35" s="25" t="s">
+      <c r="D35" s="24"/>
+      <c r="E35" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
-      <c r="R35" s="27"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="25"/>
     </row>
     <row r="36" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
-      <c r="Q36" s="27"/>
-      <c r="R36" s="27"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="25"/>
     </row>
     <row r="37" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="G37" s="28"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="27"/>
     </row>
     <row r="38" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="G38" s="30"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="30"/>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="30"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="28"/>
+      <c r="Q38" s="28"/>
+      <c r="R38" s="28"/>
     </row>
     <row r="39" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="G39" s="30"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="30"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+      <c r="P39" s="28"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="28"/>
     </row>
     <row r="40" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="G40" s="30"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="R40" s="30"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="28"/>
+      <c r="R40" s="28"/>
     </row>
     <row r="41" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+      <c r="O41" s="25"/>
+      <c r="P41" s="25"/>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="25"/>
     </row>
     <row r="42" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-      <c r="O42" s="27"/>
-      <c r="P42" s="27"/>
-      <c r="Q42" s="27"/>
-      <c r="R42" s="27"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="25"/>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="25"/>
     </row>
     <row r="43" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="27"/>
-      <c r="R43" s="27"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+      <c r="O43" s="25"/>
+      <c r="P43" s="25"/>
+      <c r="Q43" s="25"/>
+      <c r="R43" s="25"/>
     </row>
     <row r="44" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="27"/>
-      <c r="O44" s="27"/>
-      <c r="P44" s="27"/>
-      <c r="Q44" s="27"/>
-      <c r="R44" s="27"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+      <c r="O44" s="25"/>
+      <c r="P44" s="25"/>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3464,7 +3505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3477,18 +3518,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="29" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="5">
@@ -3499,10 +3540,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="30">
         <v>2007</v>
       </c>
       <c r="C3" s="2">
@@ -3510,7 +3551,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="30" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="5">
@@ -3521,10 +3562,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="30">
         <v>2009</v>
       </c>
       <c r="C5" s="2">
@@ -3532,7 +3573,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="30" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="5">
@@ -3543,10 +3584,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="30">
         <v>2011</v>
       </c>
       <c r="C7" s="2">
@@ -3554,7 +3595,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="5">
@@ -3565,10 +3606,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="30">
         <v>2013</v>
       </c>
       <c r="C9" s="2">
@@ -3576,7 +3617,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="30" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="5">
@@ -3587,10 +3628,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="30">
         <v>2015</v>
       </c>
       <c r="C11" s="2">
@@ -3598,7 +3639,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="30" t="s">
         <v>59</v>
       </c>
       <c r="B12" s="5">
@@ -3609,10 +3650,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="30">
         <v>2017</v>
       </c>
       <c r="C13" s="2">
@@ -3620,7 +3661,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="30" t="s">
         <v>59</v>
       </c>
       <c r="B14" s="5">
@@ -3631,10 +3672,10 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="30">
         <v>2019</v>
       </c>
       <c r="C15" s="2">
@@ -3647,20 +3688,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3673,186 +3715,688 @@
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="7">
-        <f>SUM(D3:D4)</f>
-        <v>0.32141306999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="31">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="31">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="33">
+        <v>1.4419999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="33">
+        <v>1.4419999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1.4419999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="33">
+        <v>1.4419999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="33">
+        <v>1.4419999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>6</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="33">
+        <v>1.4419999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="31">
+        <v>1.286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>6</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="31">
+        <v>1.286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="31">
+        <v>0.36859999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>6</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="31">
+        <v>0.36859999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D20" s="33">
+        <f>SUM(D21:D22)</f>
+        <v>0.32141306999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>6</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="33">
         <f>'Manglar total mse'!J30</f>
         <v>0.32141306999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="22" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="D22" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="7">
-        <f>SUM(D6:D7)</f>
+      <c r="D23" s="33">
+        <f>SUM(D24:D25)</f>
         <v>0.30224000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="24" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D24" s="33">
         <f>'Manglar total mse'!K30</f>
         <v>0.30224000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="25" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="D25" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26">
+        <v>143.57499999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>7</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27">
+        <v>143.57499999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>7</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29">
+        <v>96.025000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>7</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30">
+        <v>96.025000000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32">
+        <v>76.170000000000016</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>7</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33">
+        <v>76.170000000000016</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35">
+        <v>65.305200000000013</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>7</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36">
+        <v>65.305200000000013</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>7</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38">
+        <v>40.383200000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>7</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>40.383200000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>7</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>7</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41">
+        <v>24.148900000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>7</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42">
+        <v>24.148900000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>7</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>7</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="31">
-        <f>SUM(D9:D10)</f>
+      <c r="D44" s="33">
+        <f>SUM(D45:D46)</f>
         <v>34.022953079999994</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="45" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B45" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C45" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D45" s="33">
         <f>'Manglar total mse'!J31</f>
         <v>34.022953079999994</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+    <row r="46" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C46" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="D46" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C47" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="31">
-        <f>SUM(D12:D13)</f>
+      <c r="D47" s="33">
+        <f>SUM(D48:D49)</f>
         <v>28.045209</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    <row r="48" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
         <v>7</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B48" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C48" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D48" s="33">
         <f>'Manglar total mse'!K31</f>
         <v>28.045209</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+    <row r="49" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
         <v>7</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C49" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D49" s="35">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>